<commit_message>
Modificando los documentos de requerimientos y user stories
</commit_message>
<xml_diff>
--- a/Documentos/Scrum docs/User Stories.xlsx
+++ b/Documentos/Scrum docs/User Stories.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Columna</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>BKLGI-008</t>
-  </si>
-  <si>
-    <t>BKLGI-009</t>
   </si>
   <si>
     <t>BKLGI-0010</t>
@@ -279,6 +276,15 @@
     <t xml:space="preserve">SISTEMA: </t>
   </si>
   <si>
+    <t>BKLGI-0011</t>
+  </si>
+  <si>
+    <t>BKLGI-0012</t>
+  </si>
+  <si>
+    <t>BKLGI-0013</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Como </t>
     </r>
@@ -291,7 +297,65 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>vendedor</t>
+      <t xml:space="preserve">usuario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">necesito </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">poder tener una lista de contactos, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con la finalidad de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>poder saber con quienes puedo usar la aplicación.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usuario</t>
     </r>
     <r>
       <rPr>
@@ -312,7 +376,65 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">poder registrar y actualizar clientes, </t>
+      <t>poder crear, guardar, visualizar, modificar,  y eliminar mis propios horarios</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, con la finalidad de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>poder administrar éstos de manera detallada.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> necesito </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">poder comparar mi horario con los horarios de mis otros contactos, </t>
     </r>
     <r>
       <rPr>
@@ -333,8 +455,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>poder realizar una venta.</t>
-    </r>
+      <t>poder visualizar las coincidencias de horas libres y ocupadas que tengo con ellos.</t>
+    </r>
+  </si>
+  <si>
+    <t>BKLGI-0009</t>
   </si>
   <si>
     <r>
@@ -349,7 +474,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>administrador</t>
+      <t>usuario</t>
     </r>
     <r>
       <rPr>
@@ -370,7 +495,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">poder registrar y actualizar empleados, </t>
+      <t xml:space="preserve">poder crear, guardar, visualizar, modificar,  y eliminar grupos en base a mis contactos, </t>
     </r>
     <r>
       <rPr>
@@ -391,7 +516,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>poder tener un control de éstos.</t>
+      <t>poder administrar estos.</t>
     </r>
   </si>
   <si>
@@ -407,7 +532,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>vendedor</t>
+      <t>usuario</t>
     </r>
     <r>
       <rPr>
@@ -428,7 +553,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">poder generar un ticket de venta </t>
+      <t xml:space="preserve">poder agregar personas adicionales a mis grupos, </t>
     </r>
     <r>
       <rPr>
@@ -449,7 +574,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> poder brindar al cliente un comprobante de compra.</t>
+      <t xml:space="preserve"> poder encontrar nuevas concidencias con estas.</t>
     </r>
   </si>
   <si>
@@ -465,7 +590,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>administrador</t>
+      <t>usuario</t>
     </r>
     <r>
       <rPr>
@@ -486,17 +611,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">poder tener un reporte de los productos de sistema, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
+      <t xml:space="preserve">poder nombrar mis grupos de contactos, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con la finalidad de</t>
     </r>
     <r>
       <rPr>
@@ -507,7 +632,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>poder tener un control de éstos.</t>
+      <t xml:space="preserve"> poder diferenciar.</t>
     </r>
   </si>
   <si>
@@ -523,7 +648,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>administrador</t>
+      <t>usuario</t>
     </r>
     <r>
       <rPr>
@@ -544,17 +669,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>poder tener un reporte de las ventas hechas,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
+      <t xml:space="preserve">poder registrarme a la aplicación con mi cuenta de facebook, twitter, gmail, etc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con la finalidad de</t>
     </r>
     <r>
       <rPr>
@@ -565,541 +690,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>poder tener un control de éstos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vendedor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">poder registrar y/o actualizar ventas de productos, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> poder generar ingresos a la empresa.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vendedor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un listado de los productos disponibles en stock,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder realizar una venta.</t>
-    </r>
-  </si>
-  <si>
-    <t>BKLGI-0011</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>administrador</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un reporte de ventas realizadas por vendedor,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un control administrativo.</t>
-    </r>
-  </si>
-  <si>
-    <t>BKLGI-0012</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>administrador</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un listado de clientes,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un control administrativo.</t>
-    </r>
-  </si>
-  <si>
-    <t>BKLGI-0013</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>administrador</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un listado de empleados,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un control administrativo.</t>
-    </r>
-  </si>
-  <si>
-    <t>BKLGI-0014</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>administrador</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un listado de proveedores</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener un control administrativo.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>usuario del sistema</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder comparar mi horario con los horarios de mis otros contactos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder visualizar las coincidencias de horas libres y ocupadas que tengo con ellos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>usuario del sistema</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder crear, visualizar, modificar,  y eliminar mis propios horarios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder administrar éstos de manera detallada.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>usuario del sistema</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> necesito </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">poder contar con tres opciones básicas crear horarios, visualizar, y enlazar horarios, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder tener control de éstos.</t>
+      <t xml:space="preserve"> poder crearme una cuenta de forma rápida</t>
     </r>
   </si>
 </sst>
@@ -1576,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G18"/>
+  <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1185,7 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1631,7 +1222,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -1639,12 +1230,12 @@
       <c r="F5" s="5"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -1657,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -1665,12 +1256,12 @@
       <c r="F7" s="5"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -1683,7 +1274,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -1696,7 +1287,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
@@ -1704,12 +1295,12 @@
       <c r="F10" s="5"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -1722,7 +1313,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
@@ -1732,11 +1323,9 @@
     </row>
     <row r="13" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1745,11 +1334,9 @@
     </row>
     <row r="14" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1758,55 +1345,36 @@
     </row>
     <row r="15" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1836,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1852,7 +1420,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -1860,7 +1428,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1876,7 +1444,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1892,7 +1460,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>